<commit_message>
updates incidence rate and risk level
</commit_message>
<xml_diff>
--- a/Incidence sms alert/output/Sectors (BXW incidence level)-Quarterly update.xlsx
+++ b/Incidence sms alert/output/Sectors (BXW incidence level)-Quarterly update.xlsx
@@ -5,22 +5,27 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\WORK\RAB_ICT4BXW\BXW Alert initiate\Quarterly..sectors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Documents\WORK\ICT4BXW Webapp\AA_BXWAPP FINAL\AAAAAAAAAAAAAAAAAAA\autorepo\ict4bxw\Incidence sms alert\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8994" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8994" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="June" sheetId="1" r:id="rId1"/>
-    <sheet name="Sept" sheetId="2" r:id="rId2"/>
+    <sheet name="June_22 " sheetId="1" r:id="rId1"/>
+    <sheet name="Sept_22" sheetId="2" r:id="rId2"/>
+    <sheet name="Jan_23" sheetId="3" r:id="rId3"/>
+    <sheet name="Mar_23" sheetId="4" r:id="rId4"/>
+    <sheet name="June_23" sheetId="5" r:id="rId5"/>
+    <sheet name="Sept_23" sheetId="6" r:id="rId6"/>
+    <sheet name="Jan_24" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="152">
   <si>
     <t>District</t>
   </si>
@@ -437,6 +442,45 @@
   </si>
   <si>
     <t>Murambi</t>
+  </si>
+  <si>
+    <t>totalDiagnoses</t>
+  </si>
+  <si>
+    <t>totalIncidence</t>
+  </si>
+  <si>
+    <t>incidenceRate</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+  <si>
+    <t>CYUNGO</t>
+  </si>
+  <si>
+    <t>RWAZA</t>
+  </si>
+  <si>
+    <t>MUSASA</t>
+  </si>
+  <si>
+    <t>NGOMA</t>
+  </si>
+  <si>
+    <t>NYAKABUYE</t>
+  </si>
+  <si>
+    <t>MUKO</t>
+  </si>
+  <si>
+    <t>KIREHE</t>
+  </si>
+  <si>
+    <t>GATORE</t>
+  </si>
+  <si>
+    <t>NDEGO</t>
   </si>
 </sst>
 </file>
@@ -1246,11 +1290,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="4" max="4" width="15.83984375" customWidth="1"/>
+    <col min="5" max="5" width="14.578125" customWidth="1"/>
+    <col min="6" max="6" width="18.26171875" customWidth="1"/>
+    <col min="7" max="7" width="19.83984375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
@@ -2247,11 +2297,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="6" max="6" width="14.734375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" t="s">
@@ -3518,4 +3571,1343 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F63"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="15.734375" customWidth="1"/>
+    <col min="2" max="2" width="12.7890625" customWidth="1"/>
+    <col min="3" max="3" width="13.15625" customWidth="1"/>
+    <col min="4" max="4" width="12.89453125" customWidth="1"/>
+    <col min="5" max="5" width="14.47265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4">
+        <v>80</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5">
+        <v>123</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6">
+        <v>307</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0.65</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>141</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0.71</v>
+      </c>
+      <c r="F7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8">
+        <v>562</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>0.71</v>
+      </c>
+      <c r="F8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1.85</v>
+      </c>
+      <c r="F9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10">
+        <v>100</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11">
+        <v>235</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12">
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3.45</v>
+      </c>
+      <c r="F12" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13">
+        <v>28</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>3.57</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14">
+        <v>28</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>3.57</v>
+      </c>
+      <c r="F14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C15">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+      <c r="C16">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>4.3499999999999996</v>
+      </c>
+      <c r="F16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17">
+        <v>64</v>
+      </c>
+      <c r="D17">
+        <v>3</v>
+      </c>
+      <c r="E17">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18">
+        <v>86</v>
+      </c>
+      <c r="D18">
+        <v>5</v>
+      </c>
+      <c r="E18">
+        <v>5.81</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19">
+        <v>621</v>
+      </c>
+      <c r="D19">
+        <v>37</v>
+      </c>
+      <c r="E19">
+        <v>5.96</v>
+      </c>
+      <c r="F19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20">
+        <v>81</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>6.17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21">
+        <v>99</v>
+      </c>
+      <c r="D21">
+        <v>7</v>
+      </c>
+      <c r="E21">
+        <v>7.07</v>
+      </c>
+      <c r="F21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22">
+        <v>153</v>
+      </c>
+      <c r="D22">
+        <v>14</v>
+      </c>
+      <c r="E22">
+        <v>9.15</v>
+      </c>
+      <c r="F22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C23">
+        <v>341</v>
+      </c>
+      <c r="D23">
+        <v>33</v>
+      </c>
+      <c r="E23">
+        <v>9.68</v>
+      </c>
+      <c r="F23" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24">
+        <v>251</v>
+      </c>
+      <c r="D24">
+        <v>25</v>
+      </c>
+      <c r="E24">
+        <v>9.9600000000000009</v>
+      </c>
+      <c r="F24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>56</v>
+      </c>
+      <c r="B25" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25">
+        <v>70</v>
+      </c>
+      <c r="D25">
+        <v>7</v>
+      </c>
+      <c r="E25">
+        <v>10</v>
+      </c>
+      <c r="F25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26">
+        <v>327</v>
+      </c>
+      <c r="D26">
+        <v>39</v>
+      </c>
+      <c r="E26">
+        <v>11.93</v>
+      </c>
+      <c r="F26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27">
+        <v>33</v>
+      </c>
+      <c r="D27">
+        <v>4</v>
+      </c>
+      <c r="E27">
+        <v>12.12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28">
+        <v>104</v>
+      </c>
+      <c r="D28">
+        <v>13</v>
+      </c>
+      <c r="E28">
+        <v>12.5</v>
+      </c>
+      <c r="F28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="B29" t="s">
+        <v>146</v>
+      </c>
+      <c r="C29">
+        <v>23</v>
+      </c>
+      <c r="D29">
+        <v>3</v>
+      </c>
+      <c r="E29">
+        <v>13.04</v>
+      </c>
+      <c r="F29" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30">
+        <v>238</v>
+      </c>
+      <c r="D30">
+        <v>39</v>
+      </c>
+      <c r="E30">
+        <v>16.39</v>
+      </c>
+      <c r="F30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31">
+        <v>22</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+      <c r="E31">
+        <v>18.18</v>
+      </c>
+      <c r="F31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32">
+        <v>26</v>
+      </c>
+      <c r="D32">
+        <v>5</v>
+      </c>
+      <c r="E32">
+        <v>19.23</v>
+      </c>
+      <c r="F32" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>149</v>
+      </c>
+      <c r="B33" t="s">
+        <v>150</v>
+      </c>
+      <c r="C33">
+        <v>26</v>
+      </c>
+      <c r="D33">
+        <v>5</v>
+      </c>
+      <c r="E33">
+        <v>19.23</v>
+      </c>
+      <c r="F33" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34">
+        <v>115</v>
+      </c>
+      <c r="D34">
+        <v>23</v>
+      </c>
+      <c r="E34">
+        <v>20</v>
+      </c>
+      <c r="F34" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35">
+        <v>98</v>
+      </c>
+      <c r="D35">
+        <v>21</v>
+      </c>
+      <c r="E35">
+        <v>21.43</v>
+      </c>
+      <c r="F35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" t="s">
+        <v>43</v>
+      </c>
+      <c r="C36">
+        <v>182</v>
+      </c>
+      <c r="D36">
+        <v>40</v>
+      </c>
+      <c r="E36">
+        <v>21.98</v>
+      </c>
+      <c r="F36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C37">
+        <v>22</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37">
+        <v>22.73</v>
+      </c>
+      <c r="F37" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" t="s">
+        <v>46</v>
+      </c>
+      <c r="C38">
+        <v>110</v>
+      </c>
+      <c r="D38">
+        <v>26</v>
+      </c>
+      <c r="E38">
+        <v>23.64</v>
+      </c>
+      <c r="F38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" t="s">
+        <v>42</v>
+      </c>
+      <c r="C39">
+        <v>22</v>
+      </c>
+      <c r="D39">
+        <v>6</v>
+      </c>
+      <c r="E39">
+        <v>27.27</v>
+      </c>
+      <c r="F39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40">
+        <v>88</v>
+      </c>
+      <c r="D40">
+        <v>24</v>
+      </c>
+      <c r="E40">
+        <v>27.27</v>
+      </c>
+      <c r="F40" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41">
+        <v>248</v>
+      </c>
+      <c r="D41">
+        <v>69</v>
+      </c>
+      <c r="E41">
+        <v>27.82</v>
+      </c>
+      <c r="F41" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C42">
+        <v>86</v>
+      </c>
+      <c r="D42">
+        <v>26</v>
+      </c>
+      <c r="E42">
+        <v>30.23</v>
+      </c>
+      <c r="F42" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>44</v>
+      </c>
+      <c r="B43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43">
+        <v>157</v>
+      </c>
+      <c r="D43">
+        <v>48</v>
+      </c>
+      <c r="E43">
+        <v>30.57</v>
+      </c>
+      <c r="F43" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44">
+        <v>73</v>
+      </c>
+      <c r="D44">
+        <v>24</v>
+      </c>
+      <c r="E44">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="F44" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>35</v>
+      </c>
+      <c r="B45" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45">
+        <v>21</v>
+      </c>
+      <c r="D45">
+        <v>7</v>
+      </c>
+      <c r="E45">
+        <v>33.33</v>
+      </c>
+      <c r="F45" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <v>114</v>
+      </c>
+      <c r="D46">
+        <v>41</v>
+      </c>
+      <c r="E46">
+        <v>35.96</v>
+      </c>
+      <c r="F46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>28</v>
+      </c>
+      <c r="B47" t="s">
+        <v>29</v>
+      </c>
+      <c r="C47">
+        <v>71</v>
+      </c>
+      <c r="D47">
+        <v>29</v>
+      </c>
+      <c r="E47">
+        <v>40.85</v>
+      </c>
+      <c r="F47" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B48" t="s">
+        <v>33</v>
+      </c>
+      <c r="C48">
+        <v>251</v>
+      </c>
+      <c r="D48">
+        <v>103</v>
+      </c>
+      <c r="E48">
+        <v>41.04</v>
+      </c>
+      <c r="F48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" t="s">
+        <v>148</v>
+      </c>
+      <c r="C49">
+        <v>24</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+      <c r="E49">
+        <v>41.67</v>
+      </c>
+      <c r="F49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>30</v>
+      </c>
+      <c r="B50" t="s">
+        <v>31</v>
+      </c>
+      <c r="C50">
+        <v>80</v>
+      </c>
+      <c r="D50">
+        <v>35</v>
+      </c>
+      <c r="E50">
+        <v>43.75</v>
+      </c>
+      <c r="F50" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>18</v>
+      </c>
+      <c r="B51" t="s">
+        <v>26</v>
+      </c>
+      <c r="C51">
+        <v>51</v>
+      </c>
+      <c r="D51">
+        <v>23</v>
+      </c>
+      <c r="E51">
+        <v>45.1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>18</v>
+      </c>
+      <c r="B52" t="s">
+        <v>23</v>
+      </c>
+      <c r="C52">
+        <v>37</v>
+      </c>
+      <c r="D52">
+        <v>19</v>
+      </c>
+      <c r="E52">
+        <v>51.35</v>
+      </c>
+      <c r="F52" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>24</v>
+      </c>
+      <c r="B53" t="s">
+        <v>25</v>
+      </c>
+      <c r="C53">
+        <v>88</v>
+      </c>
+      <c r="D53">
+        <v>46</v>
+      </c>
+      <c r="E53">
+        <v>52.27</v>
+      </c>
+      <c r="F53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>14</v>
+      </c>
+      <c r="B54" t="s">
+        <v>20</v>
+      </c>
+      <c r="C54">
+        <v>49</v>
+      </c>
+      <c r="D54">
+        <v>28</v>
+      </c>
+      <c r="E54">
+        <v>57.14</v>
+      </c>
+      <c r="F54" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" t="s">
+        <v>147</v>
+      </c>
+      <c r="C55">
+        <v>23</v>
+      </c>
+      <c r="D55">
+        <v>14</v>
+      </c>
+      <c r="E55">
+        <v>60.87</v>
+      </c>
+      <c r="F55" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>16</v>
+      </c>
+      <c r="B56" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56">
+        <v>63</v>
+      </c>
+      <c r="D56">
+        <v>42</v>
+      </c>
+      <c r="E56">
+        <v>66.67</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>18</v>
+      </c>
+      <c r="B57" t="s">
+        <v>19</v>
+      </c>
+      <c r="C57">
+        <v>29</v>
+      </c>
+      <c r="D57">
+        <v>20</v>
+      </c>
+      <c r="E57">
+        <v>68.97</v>
+      </c>
+      <c r="F57" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" t="s">
+        <v>22</v>
+      </c>
+      <c r="C58">
+        <v>42</v>
+      </c>
+      <c r="D58">
+        <v>30</v>
+      </c>
+      <c r="E58">
+        <v>71.430000000000007</v>
+      </c>
+      <c r="F58" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" t="s">
+        <v>10</v>
+      </c>
+      <c r="B59" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59">
+        <v>36</v>
+      </c>
+      <c r="D59">
+        <v>26</v>
+      </c>
+      <c r="E59">
+        <v>72.22</v>
+      </c>
+      <c r="F59" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" t="s">
+        <v>12</v>
+      </c>
+      <c r="B60" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60">
+        <v>96</v>
+      </c>
+      <c r="D60">
+        <v>71</v>
+      </c>
+      <c r="E60">
+        <v>73.959999999999994</v>
+      </c>
+      <c r="F60" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" t="s">
+        <v>15</v>
+      </c>
+      <c r="C61">
+        <v>62</v>
+      </c>
+      <c r="D61">
+        <v>46</v>
+      </c>
+      <c r="E61">
+        <v>74.19</v>
+      </c>
+      <c r="F61" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62">
+        <v>47</v>
+      </c>
+      <c r="D62">
+        <v>36</v>
+      </c>
+      <c r="E62">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="F62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>7</v>
+      </c>
+      <c r="C63">
+        <v>46</v>
+      </c>
+      <c r="D63">
+        <v>42</v>
+      </c>
+      <c r="E63">
+        <v>91.3</v>
+      </c>
+      <c r="F63" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:F63">
+    <sortCondition ref="E1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>